<commit_message>
cleaned data according to dodgy values identified previously, summarised mean values for each trait-species combination
</commit_message>
<xml_diff>
--- a/data/traits/RF_trait_data2c.xlsx
+++ b/data/traits/RF_trait_data2c.xlsx
@@ -386,7 +386,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9178" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9191" uniqueCount="767">
   <si>
     <t>source</t>
   </si>
@@ -2687,6 +2687,21 @@
   </si>
   <si>
     <t>AUSTRAITS_dataset_56, AUSTRAITS_dataset _24</t>
+  </si>
+  <si>
+    <t>Diospyros ellipticifolia var. ebenus</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1146609X06000452</t>
+  </si>
+  <si>
+    <t>NSW flora online</t>
+  </si>
+  <si>
+    <t>http://onlinelibrary.wiley.com/doi/10.1111/j.1438-8677.2011.00528.x/full</t>
+  </si>
+  <si>
+    <t>http://hub.hku.hk/handle/10722/35055</t>
   </si>
 </sst>
 </file>
@@ -2697,7 +2712,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2914,6 +2929,14 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3267,7 +3290,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -3312,8 +3335,9 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3540,8 +3564,9 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="44"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -3575,6 +3600,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -3863,11 +3889,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2442"/>
+  <dimension ref="A1:P2449"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2411" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2433" sqref="D2433"/>
+      <pane ySplit="1" topLeftCell="A2429" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O2454" sqref="O2454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -37350,7 +37376,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="2433" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2433" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2433" t="s">
         <v>197</v>
       </c>
@@ -37369,7 +37395,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2434" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2434" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2434" t="s">
         <v>198</v>
       </c>
@@ -37388,7 +37414,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2435" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2435" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2435" t="s">
         <v>199</v>
       </c>
@@ -37407,7 +37433,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2436" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2436" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2436" s="137" t="s">
         <v>202</v>
       </c>
@@ -37426,7 +37452,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="2437" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2437" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2437" t="s">
         <v>203</v>
       </c>
@@ -37445,7 +37471,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2438" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2438" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2438" t="s">
         <v>204</v>
       </c>
@@ -37464,7 +37490,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2439" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2439" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2439" t="s">
         <v>205</v>
       </c>
@@ -37483,7 +37509,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="2440" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2440" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2440" t="s">
         <v>207</v>
       </c>
@@ -37502,7 +37528,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2441" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2441" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2441" t="s">
         <v>7</v>
       </c>
@@ -37521,7 +37547,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2442" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2442" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2442" t="s">
         <v>235</v>
       </c>
@@ -37540,12 +37566,118 @@
         <v>284</v>
       </c>
     </row>
+    <row r="2444" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2444" t="s">
+        <v>762</v>
+      </c>
+      <c r="B2444"/>
+      <c r="C2444"/>
+      <c r="D2444"/>
+      <c r="E2444"/>
+      <c r="F2444"/>
+      <c r="G2444">
+        <v>72.45</v>
+      </c>
+      <c r="H2444"/>
+      <c r="I2444">
+        <v>6</v>
+      </c>
+      <c r="J2444"/>
+      <c r="K2444">
+        <v>45.996000000000002</v>
+      </c>
+      <c r="N2444"/>
+      <c r="O2444" t="s">
+        <v>256</v>
+      </c>
+      <c r="P2444"/>
+    </row>
+    <row r="2445" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2445" t="s">
+        <v>762</v>
+      </c>
+      <c r="L2445" s="9">
+        <v>11</v>
+      </c>
+      <c r="M2445" s="9">
+        <v>2</v>
+      </c>
+      <c r="N2445" s="9">
+        <v>4</v>
+      </c>
+      <c r="O2445" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2446" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2446" s="9">
+        <v>50.86</v>
+      </c>
+      <c r="F2446" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G2446" s="9">
+        <v>93.2</v>
+      </c>
+      <c r="N2446" s="1"/>
+      <c r="O2446" s="1" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2447" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2447" s="77">
+        <v>15</v>
+      </c>
+      <c r="L2447" s="9">
+        <v>1</v>
+      </c>
+      <c r="M2447" s="9">
+        <v>12</v>
+      </c>
+      <c r="N2447" s="9">
+        <v>12</v>
+      </c>
+      <c r="O2447" s="1" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2448" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2448" s="9">
+        <v>47.44</v>
+      </c>
+      <c r="O2448" s="140" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2449" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2449" s="9">
+        <v>0.59</v>
+      </c>
+      <c r="O2449" s="1" t="s">
+        <v>766</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:N2357">
     <sortCondition ref="G1"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="O2448" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>